<commit_message>
b rith item import
</commit_message>
<xml_diff>
--- a/assets/imports/items_import_form_excel.xlsx
+++ b/assets/imports/items_import_form_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loatchoeun/Desktop/imports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/c2/assets/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>abbr</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>depreciation_account</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -408,85 +411,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:T78"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="12" max="12" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" customWidth="1"/>
-    <col min="17" max="17" width="21.5" customWidth="1"/>
-    <col min="18" max="18" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.33203125" customWidth="1"/>
-    <col min="20" max="20" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="13" max="13" width="10.5" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" customWidth="1"/>
+    <col min="18" max="18" width="21.5" customWidth="1"/>
+    <col min="19" max="19" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.33203125" customWidth="1"/>
+    <col min="21" max="21" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>